<commit_message>
work, mostly just getting parse_job_sheet workin
</commit_message>
<xml_diff>
--- a/outputs/timesheet_daily_summary.xlsx
+++ b/outputs/timesheet_daily_summary.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,18 +491,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Founders 2</t>
+          <t>Column8</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>28.5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Honorio G, Rigoberto Al-B, Rogelio M</t>
+          <t>Column1</t>
         </is>
       </c>
     </row>
@@ -512,18 +512,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GU Henle</t>
+          <t>Founders 2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>38</v>
+        <v>28.5</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Fernando V, Laurentino, Noe VL, Oscar VS</t>
+          <t>Honorio G, Rigoberto Al-B, Rogelio M</t>
         </is>
       </c>
     </row>
@@ -533,18 +533,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>HanoverSpring</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Antoine F, Carlos Al-V, Gaudencio B, Jose P, Moises P, Rata F</t>
+          <t>Fernando V, Laurentino, Noe VL, Oscar VS</t>
         </is>
       </c>
     </row>
@@ -554,18 +554,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Adalberto T, Daniel LG, Elvis T, Henry G, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
+          <t>Antoine F, Carlos Al-V, Gaudencio B, Jose P, Moises P, Rata F</t>
         </is>
       </c>
     </row>
@@ -575,18 +575,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
+          <t>Adalberto T, Daniel LG, Elvis T, Henry G, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
@@ -596,39 +596,39 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>Tidal Basin</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Jose Luis H, Juan G, Miguel A, Misael M, Pablo G, William A</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45909</v>
+        <v>45908</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ARA3A     Moorefield</t>
+          <t>Wardman</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D9" t="n">
-        <v>66.5</v>
+        <v>133</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Benito A, Daniel GS, Eric M R, Evaristo A, Henry G, Leobardo RL, Omar S</t>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Jose Luis H, Juan G, Miguel A, Misael M, Pablo G, William A</t>
         </is>
       </c>
     </row>
@@ -638,18 +638,18 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Canvas</t>
+          <t>ARA3A     Moorefield</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D10" t="n">
-        <v>9.5</v>
+        <v>66.5</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Noe VL</t>
+          <t>Benito A, Daniel GS, Eric M R, Evaristo A, Henry G, Leobardo RL, Omar S</t>
         </is>
       </c>
     </row>
@@ -659,18 +659,18 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Founders 2</t>
+          <t>Canvas</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>27</v>
+        <v>9.5</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Honorio G, Rigoberto Al-B, Rogelio M</t>
+          <t>Noe VL</t>
         </is>
       </c>
     </row>
@@ -680,18 +680,18 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GU Henle</t>
+          <t>Column13</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>28.5</v>
+        <v>9</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Fernando V, Laurentino, Oscar VS</t>
+          <t>Column1</t>
         </is>
       </c>
     </row>
@@ -701,18 +701,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>HanoverSpring</t>
+          <t>Founders 2</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
-        <v>47.5</v>
+        <v>27</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Carlos Al-V, Gaudencio B, Jose P, Moises P, Rata F</t>
+          <t>Honorio G, Rigoberto Al-B, Rogelio M</t>
         </is>
       </c>
     </row>
@@ -722,18 +722,18 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
-        <v>66.5</v>
+        <v>28.5</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Adalberto T, Daniel LG, Elvis T, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
+          <t>Fernando V, Laurentino, Oscar VS</t>
         </is>
       </c>
     </row>
@@ -743,18 +743,18 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>57</v>
+        <v>47.5</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
+          <t>Carlos Al-V, Gaudencio B, Jose P, Moises P, Rata F</t>
         </is>
       </c>
     </row>
@@ -764,60 +764,60 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D16" t="n">
-        <v>114</v>
+        <v>66.5</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Pablo G, William A</t>
+          <t>Adalberto T, Daniel LG, Elvis T, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45910</v>
+        <v>45909</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2011 Crystal</t>
+          <t>Tidal Basin</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>28.5</v>
+        <v>57</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Alejandro M S, Rigoberto Al-B, Rogelio M</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45910</v>
+        <v>45909</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BridgeDist</t>
+          <t>Wardman</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D18" t="n">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Elvis T, Evaristo A</t>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Pablo G, William A</t>
         </is>
       </c>
     </row>
@@ -827,18 +827,18 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>GU Henle</t>
+          <t>2011 Crystal</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D19" t="n">
-        <v>49.5</v>
+        <v>28.5</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Fernando V, Jose Carlos G, Laurentino, Noe VL, Oscar VS</t>
+          <t>Alejandro M S, Rigoberto Al-B, Rogelio M</t>
         </is>
       </c>
     </row>
@@ -848,18 +848,18 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>HanoverSpring</t>
+          <t>BridgeDist</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Carlos Al-V, Jose P, Moises P, Rata F</t>
+          <t>Elvis T, Evaristo A</t>
         </is>
       </c>
     </row>
@@ -869,18 +869,18 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kingstowne</t>
+          <t>Column18</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Adalberto T, Gaudencio B, Luis Enrique R, Luis Martin R, Trinidad T</t>
+          <t>Column1</t>
         </is>
       </c>
     </row>
@@ -890,18 +890,18 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Moorfield</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D22" t="n">
-        <v>67</v>
+        <v>49.5</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Benito A, Daniel GS, Daniel LG, Eric M R, Julio M, Leobardo RL, Omar S</t>
+          <t>Fernando V, Jose Carlos G, Laurentino, Noe VL, Oscar VS</t>
         </is>
       </c>
     </row>
@@ -911,18 +911,18 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D23" t="n">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
+          <t>Carlos Al-V, Jose P, Moises P, Rata F</t>
         </is>
       </c>
     </row>
@@ -932,81 +932,81 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>Kingstowne</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D24" t="n">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Pablo G, William A</t>
+          <t>Adalberto T, Gaudencio B, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45911</v>
+        <v>45910</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2011 Crystal</t>
+          <t>Moorfield</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D25" t="n">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Alejandro M S, Gerardo D, Rigoberto Al-B</t>
+          <t>Benito A, Daniel GS, Daniel LG, Eric M R, Julio M, Leobardo RL, Omar S</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45911</v>
+        <v>45910</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2011 Crystal    Yard</t>
+          <t>Tidal Basin</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Rogelio M</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45911</v>
+        <v>45910</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>GU Henle</t>
+          <t>Wardman</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D27" t="n">
-        <v>47.5</v>
+        <v>114</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Fernando V, Jose Carlos G, Laurentino, Noe VL, Oscar VS</t>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Pablo G, William A</t>
         </is>
       </c>
     </row>
@@ -1016,18 +1016,18 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>HanoverSpring</t>
+          <t>2011 Crystal</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" t="n">
-        <v>47.5</v>
+        <v>27</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Antoine F, Carlos Al-V, Jose P, Moises P, Rata F</t>
+          <t>Alejandro M S, Gerardo D, Rigoberto Al-B</t>
         </is>
       </c>
     </row>
@@ -1037,18 +1037,18 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Kingstowne</t>
+          <t>2011 Crystal    Yard</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Adalberto T, Elvis T, Gaudencio B, Julio M, Leobardo RL, Luis Enrique R, Luis Martin R, Trinidad T</t>
+          <t>Rogelio M</t>
         </is>
       </c>
     </row>
@@ -1058,18 +1058,18 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Moorefield</t>
+          <t>Column23</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Benito A, Daniel GS, Daniel LG, Eric M R, Evaristo A, Omar S</t>
+          <t>Column1</t>
         </is>
       </c>
     </row>
@@ -1079,18 +1079,18 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D31" t="n">
-        <v>66.5</v>
+        <v>47.5</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR, William A</t>
+          <t>Fernando V, Jose Carlos G, Laurentino, Noe VL, Oscar VS</t>
         </is>
       </c>
     </row>
@@ -1100,66 +1100,66 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D32" t="n">
-        <v>111</v>
+        <v>47.5</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Misael M, Pablo G</t>
+          <t>Antoine F, Carlos Al-V, Jose P, Moises P, Rata F</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45912</v>
+        <v>45911</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>Kingstowne</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D33" t="n">
-        <v>9.5</v>
+        <v>76</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Eduardo H</t>
+          <t>Adalberto T, Elvis T, Gaudencio B, Julio M, Leobardo RL, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45912</v>
+        <v>45911</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>Moorefield</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Cristobal L, Eliacim R, Jesus L, Juan G, Miguel A, Misael M, Pablo G</t>
+          <t>Benito A, Daniel GS, Daniel LG, Eric M R, Evaristo A, Omar S</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45913</v>
+        <v>45911</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1167,33 +1167,159 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D35" t="n">
-        <v>4</v>
+        <v>66.5</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Eduardo H</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR, William A</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Wardman</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>12</v>
+      </c>
+      <c r="D36" t="n">
+        <v>111</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Misael M, Pablo G</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Column28</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>24</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Column1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Tidal Basin</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Eduardo H</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45912</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Wardman</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>9</v>
+      </c>
+      <c r="D39" t="n">
+        <v>82</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Alfonso D, Andres G, Cristobal L, Eliacim R, Jesus L, Juan G, Miguel A, Misael M, Pablo G</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
         <v>45913</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Column28</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>29</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Column1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Tidal Basin</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>4</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Eduardo H</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45913</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>Wardman</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="C42" t="n">
         <v>9</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D42" t="n">
         <v>49.5</v>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>Alfonso D, Andres G, Cristobal L, Eliacim R, Jesus L, Juan G, Miguel A, Misael M, Pablo G</t>
         </is>

</xml_diff>

<commit_message>
everything seems to be workin
</commit_message>
<xml_diff>
--- a/outputs/timesheet_daily_summary.xlsx
+++ b/outputs/timesheet_daily_summary.xlsx
@@ -474,14 +474,14 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>47.5</v>
+        <v>57</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Benito A, Daniel GS, Evaristo A, Leobardo RL, Omar S</t>
+          <t>Benito A, Daniel GS, Evaristo A, Leobardo RL, Moises P, Omar S</t>
         </is>
       </c>
     </row>
@@ -491,18 +491,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Column8</t>
+          <t>Founders 2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>28.5</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Column1</t>
+          <t>Honorio G, Rigoberto Al-B, Rogelio M</t>
         </is>
       </c>
     </row>
@@ -512,18 +512,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Founders 2</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>28.5</v>
+        <v>38</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Honorio G, Rigoberto Al-B, Rogelio M</t>
+          <t>Fernando V, Laurentino, Noe VL, Oscar VS</t>
         </is>
       </c>
     </row>
@@ -533,7 +533,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GU Henle</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -544,7 +544,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Fernando V, Laurentino, Noe VL, Oscar VS</t>
+          <t>Antoine F, Carlos Al-V, Jose P, Rata F</t>
         </is>
       </c>
     </row>
@@ -554,18 +554,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>HanoverSpring</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>57</v>
+        <v>85.5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Antoine F, Carlos Al-V, Gaudencio B, Jose P, Moises P, Rata F</t>
+          <t>Adalberto T, Daniel LG, Elvis T, Gaudencio B, Henry G, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
@@ -575,18 +575,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>Tidal Basin</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Adalberto T, Daniel LG, Elvis T, Henry G, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
         </is>
       </c>
     </row>
@@ -596,39 +596,39 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>Wardman</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Jose Luis H, Juan G, Miguel A, Misael M, Pablo G, William A</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45908</v>
+        <v>45909</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>ARA3A</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Jose Luis H, Juan G, Miguel A, Misael M, Pablo G, William A</t>
+          <t>Benito A, Daniel GS, Eric M R, Evaristo A, Leobardo RL, Omar S</t>
         </is>
       </c>
     </row>
@@ -638,18 +638,18 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ARA3A     Moorefield</t>
+          <t>Founders 2</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D10" t="n">
-        <v>66.5</v>
+        <v>27</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Benito A, Daniel GS, Eric M R, Evaristo A, Henry G, Leobardo RL, Omar S</t>
+          <t>Honorio G, Rigoberto Al-B, Rogelio M</t>
         </is>
       </c>
     </row>
@@ -659,18 +659,18 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Canvas</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>9.5</v>
+        <v>38</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Noe VL</t>
+          <t>Fernando V, Laurentino, Noe VL, Oscar VS</t>
         </is>
       </c>
     </row>
@@ -680,18 +680,18 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Column13</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Column1</t>
+          <t>Antoine F, Carlos Al-V, Gaudencio B, Jose P, Moises P, Rata F</t>
         </is>
       </c>
     </row>
@@ -701,18 +701,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Founders 2</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Honorio G, Rigoberto Al-B, Rogelio M</t>
+          <t>Adalberto T, Daniel LG, Elvis T, Henry G, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
@@ -722,18 +722,18 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GU Henle</t>
+          <t>Tidal Basin</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>28.5</v>
+        <v>57</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Fernando V, Laurentino, Oscar VS</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
         </is>
       </c>
     </row>
@@ -743,81 +743,81 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>HanoverSpring</t>
+          <t>Wardman</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>47.5</v>
+        <v>133</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Carlos Al-V, Gaudencio B, Jose P, Moises P, Rata F</t>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Jose Luis H, Juan G, Miguel A, Misael M, Pablo G, William A</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45909</v>
+        <v>45910</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Rowan</t>
+          <t>ARA3A     Moorefield</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>7</v>
       </c>
       <c r="D16" t="n">
-        <v>66.5</v>
+        <v>67</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Adalberto T, Daniel LG, Elvis T, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
+          <t>Benito A, Daniel GS, Eric M R, Evaristo A, Henry G, Leobardo RL, Omar S</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45909</v>
+        <v>45910</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>Canvas</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
+          <t>Jose Carlos G, Noe VL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45909</v>
+        <v>45910</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>Founders 2</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D18" t="n">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Pablo G, William A</t>
+          <t>Alejandro M S, Honorio G, Rigoberto Al-B, Rogelio M</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2011 Crystal</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -838,7 +838,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Alejandro M S, Rigoberto Al-B, Rogelio M</t>
+          <t>Fernando V, Laurentino, Oscar VS</t>
         </is>
       </c>
     </row>
@@ -848,18 +848,18 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BridgeDist</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Elvis T, Evaristo A</t>
+          <t>Carlos Al-V, Gaudencio B, Jose P, Moises P, Rata F</t>
         </is>
       </c>
     </row>
@@ -869,18 +869,18 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Column18</t>
+          <t>Rowan</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D21" t="n">
-        <v>14</v>
+        <v>66.5</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Column1</t>
+          <t>Adalberto T, Daniel LG, Elvis T, Julio M, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
@@ -890,18 +890,18 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>GU Henle</t>
+          <t>Tidal Basin</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" t="n">
-        <v>49.5</v>
+        <v>48</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Fernando V, Jose Carlos G, Laurentino, Noe VL, Oscar VS</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
         </is>
       </c>
     </row>
@@ -911,102 +911,102 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>HanoverSpring</t>
+          <t>Wardman</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D23" t="n">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Carlos Al-V, Jose P, Moises P, Rata F</t>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Pablo G, William A</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45910</v>
+        <v>45911</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Kingstowne</t>
+          <t>2011 Crystal</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Adalberto T, Gaudencio B, Luis Enrique R, Luis Martin R, Trinidad T</t>
+          <t>Alejandro M S, Gerardo D, Rigoberto Al-B, Rogelio M</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45910</v>
+        <v>45911</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Moorfield</t>
+          <t>BridgeDist</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Benito A, Daniel GS, Daniel LG, Eric M R, Julio M, Leobardo RL, Omar S</t>
+          <t>Elvis T, Evaristo A</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45910</v>
+        <v>45911</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" t="n">
-        <v>48</v>
+        <v>47.5</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
+          <t>Fernando V, Jose Carlos G, Laurentino, Noe VL, Oscar VS</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45910</v>
+        <v>45911</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D27" t="n">
-        <v>114</v>
+        <v>47.5</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Pablo G, William A</t>
+          <t>Antoine F, Carlos Al-V, Jose P, Moises P, Rata F</t>
         </is>
       </c>
     </row>
@@ -1016,18 +1016,18 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2011 Crystal</t>
+          <t>Kingstowne</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28" t="n">
-        <v>27</v>
+        <v>47.5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Alejandro M S, Gerardo D, Rigoberto Al-B</t>
+          <t>Adalberto T, Gaudencio B, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
@@ -1037,18 +1037,18 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2011 Crystal    Yard</t>
+          <t>Moorefield</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D29" t="n">
-        <v>9</v>
+        <v>66.5</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Rogelio M</t>
+          <t>Benito A, Daniel GS, Daniel LG, Eric M R, Julio M, Leobardo RL, Omar S</t>
         </is>
       </c>
     </row>
@@ -1058,18 +1058,18 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Column23</t>
+          <t>Tidal Basin</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D30" t="n">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Column1</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR</t>
         </is>
       </c>
     </row>
@@ -1079,123 +1079,123 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>GU Henle</t>
+          <t>Wardman</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D31" t="n">
-        <v>47.5</v>
+        <v>130</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Fernando V, Jose Carlos G, Laurentino, Noe VL, Oscar VS</t>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Jose Luis H, Juan G, Miguel A, Misael M, Pablo G, William A</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>HanoverSpring</t>
+          <t>2011 Crystal</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D32" t="n">
-        <v>47.5</v>
+        <v>27</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Antoine F, Carlos Al-V, Jose P, Moises P, Rata F</t>
+          <t>Alejandro M S, Gerardo D, Rigoberto Al-B</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Kingstowne</t>
+          <t>2011 Crystal    Yard</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Adalberto T, Elvis T, Gaudencio B, Julio M, Leobardo RL, Luis Enrique R, Luis Martin R, Trinidad T</t>
+          <t>Rogelio M</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Moorefield</t>
+          <t>Canvas, Yard</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>57</v>
+        <v>9.5</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Benito A, Daniel GS, Daniel LG, Eric M R, Evaristo A, Omar S</t>
+          <t>Honorio G</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>GU Henle</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D35" t="n">
-        <v>66.5</v>
+        <v>47.5</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR, William A</t>
+          <t>Fernando V, Jose Carlos G, Laurentino, Noe VL, Oscar VS</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>HanoverSpring</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D36" t="n">
-        <v>111</v>
+        <v>47.5</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Misael M, Pablo G</t>
+          <t>Antoine F, Carlos Al-V, Jose P, Moises P, Rata F</t>
         </is>
       </c>
     </row>
@@ -1205,18 +1205,18 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Column28</t>
+          <t>Kingstowne</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D37" t="n">
-        <v>24</v>
+        <v>78.5</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Column1</t>
+          <t>Adalberto T, Elvis T, Gaudencio B, Julio M, Leobardo RL, Luis Enrique R, Luis Martin R, Trinidad T</t>
         </is>
       </c>
     </row>
@@ -1226,18 +1226,18 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tidal Basin</t>
+          <t>Moorefield</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D38" t="n">
-        <v>9.5</v>
+        <v>66.5</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Eduardo H</t>
+          <t>Benito A, Daniel GS, Daniel LG, Eric M R, Evaristo A, Henry G, Omar S</t>
         </is>
       </c>
     </row>
@@ -1247,39 +1247,39 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Wardman</t>
+          <t>Tidal Basin</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D39" t="n">
-        <v>82</v>
+        <v>66.5</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Alfonso D, Andres G, Cristobal L, Eliacim R, Jesus L, Juan G, Miguel A, Misael M, Pablo G</t>
+          <t>Alberto R, Danis BA, Eduardo H, Feliciano R, Isidro M, Juan HR, William A</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45913</v>
+        <v>45912</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Column28</t>
+          <t>Wardman</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D40" t="n">
-        <v>29</v>
+        <v>110.5</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Column1</t>
+          <t>Alfonso D, Andres G, Benny S, Carlos G, Cristobal L, Diego R, Eliacim R, Jesus L, Juan G, Miguel A, Misael M, Pablo G</t>
         </is>
       </c>
     </row>

</xml_diff>